<commit_message>
more progress -> input modeling should start model translation
</commit_message>
<xml_diff>
--- a/data/Inspector22.xlsx
+++ b/data/Inspector22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian\Desktop\SYSC 4005 Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AF8C8D-7F9F-45BA-8858-1D5AA1C39266}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769801FF-3709-436B-B142-DE2B87CDCE87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14880" yWindow="4350" windowWidth="26355" windowHeight="16410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6045" yWindow="4590" windowWidth="26355" windowHeight="16410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -475,7 +475,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>